<commit_message>
Added new attribute: Component
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
+++ b/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\bosch\UniDeb2017-1\UniDebAutomatedCar\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GH\UniDeb2017-1\UniDebAutomatedCar\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,10 +15,10 @@
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Requirement!$A$2:$H$12</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="0">Requirement!$A$2:$H$2</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="0">Requirement!$A$2:$H$12</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="0">Requirement!$A$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Requirement!$A$2:$I$12</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">Requirement!$A$2:$I$2</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="0">Requirement!$A$2:$I$12</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="0">Requirement!$A$2:$I$2</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="73">
   <si>
     <t>UNIDEB Requirements</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>UNIDEB_24</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>HMI</t>
   </si>
 </sst>
 </file>
@@ -412,11 +421,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -448,6 +454,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -798,626 +810,703 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK26"/>
+  <dimension ref="A1:AML26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="81.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="49.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="98.28515625" style="3" customWidth="1"/>
-    <col min="9" max="1025" width="9.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="98.28515625" style="2" customWidth="1"/>
+    <col min="10" max="1026" width="9.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="H11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="H12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="H14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="H15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="H16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="H17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="H18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="H19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="H20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="H23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="H24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="H25" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="D26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H12"/>
+  <autoFilter ref="A2:I12"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1"/>

</xml_diff>

<commit_message>
[https://trello.com/c/RpCLefE2] Visualisation of court window
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
+++ b/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="88">
   <si>
     <t>UNIDEB Requirements</t>
   </si>
@@ -249,6 +249,51 @@
   </si>
   <si>
     <t>HMI</t>
+  </si>
+  <si>
+    <t>VISU</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/RpCLefE2/16-rd-visualisation</t>
+  </si>
+  <si>
+    <t>UNIDEB_25</t>
+  </si>
+  <si>
+    <t>UNIDEB_26</t>
+  </si>
+  <si>
+    <t>UNIDEB_27</t>
+  </si>
+  <si>
+    <t>UNIDEB_28</t>
+  </si>
+  <si>
+    <t>Visualisation of court window</t>
+  </si>
+  <si>
+    <t>The window displaying the court shall display the whole map (background bitmap).</t>
+  </si>
+  <si>
+    <t>The window should be resizable.</t>
+  </si>
+  <si>
+    <t>Blank area should be filled with solid (default) color.</t>
+  </si>
+  <si>
+    <t>At start up, the window should be initialized with the window size of 800x600 px.</t>
+  </si>
+  <si>
+    <t>UNIDEB_29</t>
+  </si>
+  <si>
+    <t>UNIDEB_30</t>
+  </si>
+  <si>
+    <t>The court (map) shall keep its ratio in the window, but fit to the window (in larger dimension of the map).</t>
   </si>
 </sst>
 </file>
@@ -454,11 +499,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -810,11 +855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML26"/>
+  <dimension ref="A1:AML32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I1"/>
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,17 +877,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -941,7 +986,7 @@
       <c r="E5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1500,6 +1545,162 @@
         <v>42</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[RD] Powertrain System - added requirements to the req doc
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
+++ b/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GH\UniDeb2017-1\UniDebAutomatedCar\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\school\bosch\gitrepo\UniDebAutomatedCar\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="138">
   <si>
     <t>UNIDEB Requirements</t>
   </si>
@@ -294,6 +294,162 @@
   </si>
   <si>
     <t>The court (map) shall keep its ratio in the window, but fit to the window (in larger dimension of the map).</t>
+  </si>
+  <si>
+    <t>Powertrain System RD Team 2, Sprint 1</t>
+  </si>
+  <si>
+    <t>I will use the abbreviation PS for Powertrain System</t>
+  </si>
+  <si>
+    <t>When the PS receive a Gear position signal (id 7) the value shoud be saved (if the following conditions meet) and from then it shall be deemed that the car is in that gear.</t>
+  </si>
+  <si>
+    <t>If the car's speed is 0 km/h then the saveable gear positions are: P, R, N, D (for the meaning of saveable see the requirement above)</t>
+  </si>
+  <si>
+    <t>If the car's speed is bigger than 0 km/h forwards ( so the car is moving forward direction) then the only saveable gear positions are N and D</t>
+  </si>
+  <si>
+    <t>Every time if the received gear position signal's value is equals to the currently saved one (eg the driver pressed D twice or more consequently) then the signal shall not take effect on the gear positions</t>
+  </si>
+  <si>
+    <t>If the car's speed is bigger than 0 km/h backwards (so the car is moving bacward direction) then the only saveable gear positions are N and R</t>
+  </si>
+  <si>
+    <t>If the PS receive a Headlight signal (id  10) then it should save the received value.</t>
+  </si>
+  <si>
+    <t>The default value of the Headlight shall be false (so by default, the headlights are turned off)</t>
+  </si>
+  <si>
+    <t>The default value of the Gear position shall be P (so at the beginning of the application the car should be in P gear)</t>
+  </si>
+  <si>
+    <t>The default value of the Steering wheel angle shall be 0°</t>
+  </si>
+  <si>
+    <t>When the PS receive a Steering wheel angle signal (id 6) then the received value should be added to the saved one until it reches the minimum (-720°) or the maximum (720°) value. When the value after the addition exceeds the minimum value, the value should be the minimum. When the value after the addition exceeds the maximum value, the value shoud be the maximum.</t>
+  </si>
+  <si>
+    <t>The default value of the Indicator shall be 0 (NONE) at the beginning of the application</t>
+  </si>
+  <si>
+    <t>When the PS receive an Indicator signal (id 3) the logical value shoud be saved (if the following conditions meet)</t>
+  </si>
+  <si>
+    <t>Every time if the received Indicator signal's value is equals to the currently saved one (eg the currently saved is 1 (RIGHT) and the received is also 1 (RIGHT) ) then the signal shall not take effect on the indicator's saved value (nothing should happen)</t>
+  </si>
+  <si>
+    <t>If the PS receive an Indicator signal with the value of 1 (RIGHT) the right indicator should and only the right should start to blink (with 60Hz) and the left indicator shall be turned off.</t>
+  </si>
+  <si>
+    <t>If the PS receive an Indicator signal with the value of 2 (LEFT) the left indicator should and only the ledt should start to blink (with 60Hz) and the right indicator shall be turned off.</t>
+  </si>
+  <si>
+    <t>If the PS receive an Indicator signal with the value of 0 (NONE) then both indicators shall be turned off (it should not blink)</t>
+  </si>
+  <si>
+    <t>If the PS receive an Indicator signal  with the value of 3 (EMERGENCY) both left and right indicators should start to blink in synchronized (both turn on and off at the same time while blinking) (with 60Hz)</t>
+  </si>
+  <si>
+    <t>If the PS receive a Gas pedal position signal (id 7) and the car is in P gear (see above) then the received signal should not take any effect.</t>
+  </si>
+  <si>
+    <t>If the PS receive a Gas pedal position signal and the car is in N gear then the car motor's rpm should be calculated based on the received signal's value (which is in percentage) (eg if the received signal value is 50% then the rpm should be the 50% of the maximum rpm value) and this calculated value should be considered when the PS sends the motor rpm signal (id 9)</t>
+  </si>
+  <si>
+    <t>If the PS receive a Gas pedal position signal and the car is in D gear then the car motor's rpm should be calculated based on the received signal's value (which is in percentage) (eg if the received signal value is 50% then the rpm should be the 50% of the maximum rpm value) and this calculated value should be considered when the PS sends the motor rpm signal (id 9) and the following also has to be done:
+Based on the saved steering wheel angle the car should start to accelerate with increasing the speed of the car to forward direction and this should be done by calculating the car position x and y values, the car angle value and the car's speed and sending these values by signals to the VirtualFunctionBus
+The acceleration should continue while receiving the signal and when the signal is not received anymore, the acceleration should stop and the car should gradually slow down until it reaches the speed of 0 km/h.
+The car's speed should not exceed the maximum of 120 km/h</t>
+  </si>
+  <si>
+    <t>If the PS receive a Gas pedal position signal and the car is in R gear then the car motor's rpm should be calculated based on the received signal's value (which is in percentage) (eg if the received signal value is 50% then the rpm should be the 50% of the maximum rpm value) and this calculated value should be considered when the PS sends the motor rpm signal (id 9) and the following also has to be done:
+Based on the saved steering wheel angle the car should start to accelerate with increasing the speed of the car to bacward direction and this should be done by calculating the car position x and y values, the car angle value and the car's speed and sending these values by signals to the VirtualFunctionBus
+The acceleration should continue while receiving the signal and when the signal is not received anymore, the acceleration should stop and the car should gradually slow down until it reaches the speed of 0 km/h.
+The car's speed should not exceed the maximum of 120 km/h</t>
+  </si>
+  <si>
+    <t>If the PS receive a Brake pedal position signal (id 5) and the car's speed is bigger than 0 km/h then the car's speed should be decreased by the third of the current speed until it reaches the 0 km/h speed. If the car's speed is 0 km/h then the brake pedal position signal should not take any effect.</t>
+  </si>
+  <si>
+    <t>UNIDEB_31</t>
+  </si>
+  <si>
+    <t>UNIDEB_32</t>
+  </si>
+  <si>
+    <t>UNIDEB_33</t>
+  </si>
+  <si>
+    <t>UNIDEB_34</t>
+  </si>
+  <si>
+    <t>UNIDEB_35</t>
+  </si>
+  <si>
+    <t>UNIDEB_36</t>
+  </si>
+  <si>
+    <t>UNIDEB_37</t>
+  </si>
+  <si>
+    <t>UNIDEB_38</t>
+  </si>
+  <si>
+    <t>UNIDEB_39</t>
+  </si>
+  <si>
+    <t>UNIDEB_40</t>
+  </si>
+  <si>
+    <t>UNIDEB_41</t>
+  </si>
+  <si>
+    <t>UNIDEB_42</t>
+  </si>
+  <si>
+    <t>UNIDEB_43</t>
+  </si>
+  <si>
+    <t>UNIDEB_44</t>
+  </si>
+  <si>
+    <t>UNIDEB_45</t>
+  </si>
+  <si>
+    <t>UNIDEB_46</t>
+  </si>
+  <si>
+    <t>UNIDEB_47</t>
+  </si>
+  <si>
+    <t>UNIDEB_48</t>
+  </si>
+  <si>
+    <t>UNIDEB_49</t>
+  </si>
+  <si>
+    <t>UNIDEB_50</t>
+  </si>
+  <si>
+    <t>UNIDEB_51</t>
+  </si>
+  <si>
+    <t>UNIDEB_52</t>
+  </si>
+  <si>
+    <t>UNIDEB_53</t>
+  </si>
+  <si>
+    <t>UNIDEB_54</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/htzBlck2/6-rd-powertrain-system</t>
+  </si>
+  <si>
+    <t>Powertrain System</t>
   </si>
 </sst>
 </file>
@@ -511,8 +667,36 @@
     <cellStyle name="Magyarázó szöveg" xfId="2" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -855,11 +1039,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML32"/>
+  <dimension ref="A1:AML56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33:G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,6 +1888,630 @@
         <v>14</v>
       </c>
     </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:I12"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Modified the commMatrix and RD document. Added the Radar Signal components. https://trello.com/c/vRSewHge
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
+++ b/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
@@ -11,11 +11,12 @@
     <sheet name="Requirement" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Requirement!$A$2:$I$12</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Requirement!$A$2:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Requirement!$A$2:$I$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">Requirement!$A$2:$I$12</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">Requirement!$A$2:$I$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Requirement!$A$2:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Requirement!$A$2:$I$12</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="169">
   <si>
     <t xml:space="preserve">UNIDEB Requirements</t>
   </si>
@@ -447,6 +448,101 @@
   </si>
   <si>
     <t xml:space="preserve">If the PS receive a Brake pedal position signal (id 5) and the car's speed is bigger than 0 km/h then the car's speed should be decreased by the third of the current speed until it reaches the 0 km/h speed. If the car's speed is 0 km/h then the brake pedal position signal should not take any effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radar Sensor Requirements for Sprint2 (Team1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trello.com/c/vRSewHge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radar Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Radar Sensor should be able to detect up to 5 objects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Radar Sensor should be able to filter out non relevant objects if there are too many objects in the filed of view of the sensor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Radar Sensor should be able to detect the following objects in the virtual world: (car,  pedestrian, cyclist, tree)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Radar Sensor should be configurable. The default sensor configuration should be:
+Sensor range: 20-250m
+Sensor field of view: 10-85 degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should be able to calculate the longitudinal relative velocity X of a dynamic object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should send the Longitudinal VRX Signal of a dynamic object if it is in the sensor’s active area via  (Signal ID 11).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should be able to calculate the longitudinal distance from ego.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should send the Longitudinal EGO Signal of an object if it is in the sensor’s active area via  (Signal ID 12).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should be able to calculate the lateral relative velocity Y of a dynamic object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should send the Lateral VRY Signal of a dynamic object if it is in the sensor’s active area via  (Signal ID 13).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should be able to calculate the lateral distance from ego.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sensor should send the Lateral EGO Signal of an object if it is in the sensor’s active area via  (Signal ID 14).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Radar Sensor should send the Object Size of a detected object via (Signal ID 15).</t>
   </si>
 </sst>
 </file>
@@ -468,19 +564,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -588,18 +681,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -807,7 +900,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -862,6 +955,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -970,12 +1067,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -983,13 +1080,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="81.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="49.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="98.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="3" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="3" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2444,8 +2541,372 @@
         <v>15</v>
       </c>
     </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:I12"/>
+  <autoFilter ref="A2:I70"/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updated the CommMatrix and Requirements documents with new TSR findings.
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
+++ b/UniDebAutomatedCar/doc/UniDebAutomCar2017-1_Requirements.xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_1" vbProcedure="false">Requirement!$A$2:$I$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Requirement!$A$2:$I$12</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Requirement!$A$2:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Requirement!$A$2:$I$12</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="220">
   <si>
     <t xml:space="preserve">UNIDEB Requirements</t>
   </si>
@@ -681,6 +682,30 @@
   </si>
   <si>
     <t xml:space="preserve">The TSR should send the most relevant speed limit to the ACC using the MOST RELEVANT SPEED LIMIT Signal (Signal id: 22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the driver disables the TSR system it should reset it’s accumulated data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a sign is enabled but the TSR system receives a sign that should cancel out the enabled sign the TSR system should send a disable signal via DON’T SHOW SUPPLEMENTAL SIGNS ON IC Signal (Signal id: 28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The TSR should be able to disable certain signs based on elapsed time. In our case the “no speed limit” sign should get disables after a while.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDEB_89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cancel out signal for the speed limit sign should be the MOST RELEVANT SPEED LIMIT with data of 0.</t>
   </si>
 </sst>
 </file>
@@ -702,19 +727,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -1194,15 +1216,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>165600</xdr:colOff>
+      <xdr:colOff>165960</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5172480</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1215,8 +1237,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1515960" y="35011800"/>
-          <a:ext cx="5006880" cy="4173840"/>
+          <a:off x="1516320" y="35046360"/>
+          <a:ext cx="5006520" cy="4173120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1236,12 +1258,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F112" activeCellId="0" sqref="F112"/>
+      <selection pane="bottomLeft" activeCell="C112" activeCellId="0" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3504,10 +3526,110 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3521,6 +3643,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" display="https://trello.com/c/I705RNQO/1-demo-task-1"/>
+    <hyperlink ref="E112" r:id="rId2" display="https://trello.com/c/sjrJZ7jM"/>
+    <hyperlink ref="E113" r:id="rId3" display="https://trello.com/c/sjrJZ7jM"/>
+    <hyperlink ref="E114" r:id="rId4" display="https://trello.com/c/sjrJZ7jM"/>
+    <hyperlink ref="E115" r:id="rId5" display="https://trello.com/c/sjrJZ7jM"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3529,6 +3655,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>